<commit_message>
refactor: change file main
</commit_message>
<xml_diff>
--- a/src/demo_app/detection_data.xlsx
+++ b/src/demo_app/detection_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,6 +483,66 @@
         </is>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>175.5185207047189</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>2025-05-09 04:17:38</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250509_041738.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>175.5185207047189</v>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>2025-05-09 04:18:38</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250509_041838.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>175.5185207047189</v>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>2025-05-09 04:20:59</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250509_042059.jpg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: add demo app thread work
</commit_message>
<xml_diff>
--- a/src/demo_app/detection_data.xlsx
+++ b/src/demo_app/detection_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,6 +543,1006 @@
         </is>
       </c>
     </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>204.652511051006</v>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>2025-05-19 02:39:58</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_023958.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>248.7526131883264</v>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>2025-05-19 02:40:32</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_024032.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>226.0683822623496</v>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>2025-05-19 02:43:17</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_024317.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>225.1203917133164</v>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>2025-05-19 02:43:22</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_024322.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>241.3079945388218</v>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>2025-05-19 02:43:26</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_024326.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>2025-05-19 02:58:32</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_025831.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>2025-05-19 02:58:34</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_025834.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>2025-05-19 02:58:43</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_025843.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>207.4476860651996</v>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>2025-05-19 02:58:59</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_025859.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:03:38</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_030338.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B17" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:03:59</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_030359.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B18" t="n">
+        <v>226.0683822623496</v>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:04:09</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_030409.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B19" t="n">
+        <v>180.003966151586</v>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:04:13</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_030413.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B20" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:04:17</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_030417.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B21" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:04:44</t>
+        </is>
+      </c>
+      <c r="D21" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_030444.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B22" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:05:32</t>
+        </is>
+      </c>
+      <c r="D22" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_030532.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B23" t="n">
+        <v>183.4188157255659</v>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:05:48</t>
+        </is>
+      </c>
+      <c r="D23" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_030548.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B24" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:14:44</t>
+        </is>
+      </c>
+      <c r="D24" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_031444.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B25" t="n">
+        <v>170.8412294635021</v>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:14:50</t>
+        </is>
+      </c>
+      <c r="D25" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_031450.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B26" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:18:08</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_031807.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B27" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:18:41</t>
+        </is>
+      </c>
+      <c r="D27" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_031841.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B28" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:19:02</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_031902.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B29" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:21:05</t>
+        </is>
+      </c>
+      <c r="D29" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_032105.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B30" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:21:38</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_032138.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B31" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:21:55</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_032154.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B32" t="n">
+        <v>207.4476860651996</v>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:22:16</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_032216.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B33" t="n">
+        <v>186.4100593226939</v>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:44:39</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_034438.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B34" t="n">
+        <v>181.1718722367544</v>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:44:56</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_034456.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B35" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:53:33</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_035333.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B36" t="n">
+        <v>170.8412294635021</v>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:53:46</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_035346.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B37" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:54:59</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_035458.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B38" t="n">
+        <v>244.5786280192995</v>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:55:17</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_035517.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B39" t="n">
+        <v>181.5291748272072</v>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>2025-05-19 03:58:34</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_035834.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B40" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>2025-05-19 04:00:51</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_040051.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B41" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>2025-05-19 04:01:39</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_040139.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B42" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>2025-05-19 04:04:11</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_040411.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B43" t="n">
+        <v>213.6053904521876</v>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>2025-05-19 04:04:21</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_040421.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B44" t="n">
+        <v>214.076660380549</v>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>2025-05-19 04:05:14</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_040514.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B45" t="n">
+        <v>214.076660380549</v>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>2025-05-19 04:05:38</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_040538.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B46" t="n">
+        <v>214.076660380549</v>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>2025-05-19 04:05:48</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_040548.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B47" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>2025-05-19 04:05:52</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_040552.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B48" t="n">
+        <v>249.0076578816493</v>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>2025-05-19 04:05:58</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_040558.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B49" t="n">
+        <v>230.2315755659384</v>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>2025-05-19 04:06:05</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_040604.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B50" t="n">
+        <v>241.5044006555312</v>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>2025-05-19 04:06:09</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_040609.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B51" t="n">
+        <v>241.5044006555312</v>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>2025-05-19 04:13:37</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_041337.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B52" t="n">
+        <v>241.5044006555312</v>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>2025-05-19 04:17:39</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_041736.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B53" t="n">
+        <v>241.5044006555312</v>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>2025-05-19 04:18:16</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_041816.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B54" t="n">
+        <v>241.5044006555312</v>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>2025-05-19 04:18:25</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_041825.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B55" t="n">
+        <v>214.076660380549</v>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>2025-05-19 04:18:46</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_041843.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B56" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>2025-05-19 04:24:59</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250519_042458.jpg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
feat: demo tesst 1
</commit_message>
<xml_diff>
--- a/src/demo_app/detection_data.xlsx
+++ b/src/demo_app/detection_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1543,6 +1543,26 @@
         </is>
       </c>
     </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B57" t="n">
+        <v>185.8060249923673</v>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>2025-05-21 01:18:50</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>/home/anodi108/Desktop/project/Do_An_Tot_Nghiep/DATN_PhamDangDong/DATN_PhamDangDong/resource/data/data_result/image_20250521_011847.jpg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
docs: add datn final
</commit_message>
<xml_diff>
--- a/src/demo_app/detection_data.xlsx
+++ b/src/demo_app/detection_data.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1583,6 +1583,86 @@
         </is>
       </c>
     </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B59" t="n">
+        <v>181.5</v>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>2025-06-04 14:46:15</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>/mnt/d/project/DATN/DATN_PhamDangDong/resource/data/data_result/image_20250604_144608.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B60" t="n">
+        <v>162.86</v>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>2025-06-05 00:15:30</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>/mnt/d/project/DATN/DATN_PhamDangDong/resource/data/data_result/image_20250605_001523.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B61" t="n">
+        <v>161.76</v>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>2025-06-05 00:51:04</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>/mnt/d/project/DATN/DATN_PhamDangDong/resource/data/data_result/image_20250605_005055.jpg</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>HaUI</t>
+        </is>
+      </c>
+      <c r="B62" t="n">
+        <v>175</v>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>2025-06-05 01:13:52</t>
+        </is>
+      </c>
+      <c r="D62" t="inlineStr">
+        <is>
+          <t>/mnt/d/project/DATN/DATN_PhamDangDong/resource/data/data_result/image_20250605_011345.jpg</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>